<commit_message>
Se ajustaron columnas, agregaron titulos y bordes
</commit_message>
<xml_diff>
--- a/NRFM_Auditoria/NRFM_Auditoria/bin/Debug/net8.0-windows/Extracciones/4-2024/BERNABE ESPADA.xlsx
+++ b/NRFM_Auditoria/NRFM_Auditoria/bin/Debug/net8.0-windows/Extracciones/4-2024/BERNABE ESPADA.xlsx
@@ -16,7 +16,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:si>
+    <x:t>NR Finance Mexico</x:t>
+  </x:si>
+  <x:si>
     <x:t>EKIP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Certificacion de usuarios 2024</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Reporte de usuarios</x:t>
   </x:si>
   <x:si>
     <x:t>ALVARO BALAAM NOEL ROSILLO MORALES</x:t>
@@ -59,10 +68,18 @@
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="1">
+  <x:fonts count="2">
     <x:font>
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:b/>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="16"/>
       <x:color rgb="FF000000"/>
       <x:name val="Calibri"/>
       <x:family val="2"/>
@@ -76,7 +93,7 @@
       <x:patternFill patternType="gray125"/>
     </x:fill>
   </x:fills>
-  <x:borders count="1">
+  <x:borders count="2">
     <x:border diagonalUp="0" diagonalDown="0">
       <x:left style="none">
         <x:color rgb="FF000000"/>
@@ -88,6 +105,23 @@
         <x:color rgb="FF000000"/>
       </x:top>
       <x:bottom style="none">
+        <x:color rgb="FF000000"/>
+      </x:bottom>
+      <x:diagonal style="none">
+        <x:color rgb="FF000000"/>
+      </x:diagonal>
+    </x:border>
+    <x:border diagonalUp="0" diagonalDown="0">
+      <x:left style="thin">
+        <x:color rgb="FF000000"/>
+      </x:left>
+      <x:right style="thin">
+        <x:color rgb="FF000000"/>
+      </x:right>
+      <x:top style="thin">
+        <x:color rgb="FF000000"/>
+      </x:top>
+      <x:bottom style="thin">
         <x:color rgb="FF000000"/>
       </x:bottom>
       <x:diagonal style="none">
@@ -95,13 +129,27 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="1">
+  <x:cellStyleXfs count="3">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="1">
+  <x:cellXfs count="3">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -405,65 +453,93 @@
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:cols>
+    <x:col min="1" max="1" width="4.853482" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="39.139196" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="8.424911" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="40.424911" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="24.139196" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="16.567768" style="0" customWidth="1"/>
+  </x:cols>
   <x:sheetData>
+    <x:row r="1" spans="1:6">
+      <x:c r="D1" s="1" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:6">
+      <x:c r="D2" s="1" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:6">
+      <x:c r="D3" s="1" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6">
+      <x:c r="D4" s="1" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
     <x:row r="5" spans="1:6">
-      <x:c r="A5" s="0" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B5" s="0" t="s">
+      <x:c r="A5" s="2" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C5" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="D5" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="E5" s="0" t="s">
+      <x:c r="B5" s="2" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="F5" s="0" t="s">
+      <x:c r="C5" s="2" t="s">
         <x:v>5</x:v>
       </x:c>
+      <x:c r="D5" s="2" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="E5" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="F5" s="2" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="6" spans="1:6">
-      <x:c r="A6" s="0" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B6" s="0" t="s">
+      <x:c r="A6" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B6" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C6" s="2" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D6" s="2" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="C6" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D6" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="E6" s="0" t="s">
+      <x:c r="E6" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F6" s="2" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="F6" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
     </x:row>
     <x:row r="7" spans="1:6">
-      <x:c r="A7" s="0" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B7" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="C7" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="D7" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="E7" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="F7" s="0" t="s">
-        <x:v>5</x:v>
+      <x:c r="A7" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B7" s="2" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C7" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D7" s="2" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="E7" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F7" s="2" t="s">
+        <x:v>8</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>